<commit_message>
Ficheros de configuración actualizados con la nueva columna.
</commit_message>
<xml_diff>
--- a/EjerciciosLog/PrezConfig2.xlsx
+++ b/EjerciciosLog/PrezConfig2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sal8b\OneDrive\Escritorio\LibreriaMoodleAnalisis\EjerciciosLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE32CDB8-E1CB-47C6-B73C-8EF179D87049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CADB49-04CC-45E6-8426-0B8B55B350FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="4350" windowWidth="10155" windowHeight="4800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Nombre completo del usuario</t>
   </si>
   <si>
+    <t>Incluido</t>
+  </si>
+  <si>
     <t>CUADRIELLO GALDÓS, ÁNGELA</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>CUEVAS RODRIGUEZ, SARA</t>
@@ -464,107 +470,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A15" sqref="A15:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -578,66 +625,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fichero actualizado para pasar los tests.
</commit_message>
<xml_diff>
--- a/EjerciciosLog/PrezConfig2.xlsx
+++ b/EjerciciosLog/PrezConfig2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sal8b\OneDrive\Escritorio\LibreriaMoodleAnalisis\EjerciciosLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CADB49-04CC-45E6-8426-0B8B55B350FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E179FC5-2B1E-41B9-A72A-AE2463410F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Nombre completo del usuario</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,20 +594,32 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>